<commit_message>
new regressions for distribution analysis
</commit_message>
<xml_diff>
--- a/regression results tables/regression charts.xlsx
+++ b/regression results tables/regression charts.xlsx
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Debasmita/Desktop/code-switching/regression results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93113B2D-AADC-604F-9477-BC9CA47C7C52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF1C922-B17F-CD4A-8B27-3703A607AECF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" activeTab="1" xr2:uid="{3CBD741F-C181-E74B-9D9F-C91ED02C2865}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" activeTab="2" xr2:uid="{3CBD741F-C181-E74B-9D9F-C91ED02C2865}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="cs-1 v. cs-2" sheetId="2" r:id="rId2"/>
+    <sheet name="cs-2 v. non_cs" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'cs-2 v. non_cs'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'cs-2 v. non_cs'!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'cs-2 v. non_cs'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'cs-2 v. non_cs'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'cs-2 v. non_cs'!$B$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'cs-2 v. non_cs'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'cs-2 v. non_cs'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">'cs-2 v. non_cs'!$B$1</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">'cs-2 v. non_cs'!$B$2:$B$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="22">
   <si>
     <t>coef</t>
   </si>
@@ -1303,7 +1315,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>2.1699999999999997E-2</c:v>
+                    <c:v>5.9000000000000163E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>1.04E-2</c:v>
@@ -1312,13 +1324,13 @@
                     <c:v>9.3000000000000027E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.0000000000000165E-4</c:v>
+                    <c:v>8.3999999999999631E-3</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>6.4000000000000029E-3</c:v>
+                    <c:v>8.4000000000000047E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.8000000000000004E-3</c:v>
+                    <c:v>7.3000000000000009E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1330,7 +1342,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>2.23E-2</c:v>
+                    <c:v>5.0999999999999934E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>1.06E-2</c:v>
@@ -1339,13 +1351,13 @@
                     <c:v>8.6999999999999959E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.9999999999999923E-4</c:v>
+                    <c:v>8.6000000000001631E-3</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.5999999999999939E-3</c:v>
+                    <c:v>7.5999999999999956E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>3.2000000000000015E-3</c:v>
+                    <c:v>7.6999999999999985E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1397,7 +1409,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-3.7699999999999997E-2</c:v>
+                  <c:v>0.55510000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-1.34E-2</c:v>
@@ -1406,13 +1418,13 @@
                   <c:v>3.7699999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3700000000000001E-2</c:v>
+                  <c:v>1.0256000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8.6400000000000005E-2</c:v>
+                  <c:v>-0.1144</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.78E-2</c:v>
+                  <c:v>-4.4299999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,6 +1600,477 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Regression Coefficients for CS-2 (coded 1) v. non-code-switched (coded 0)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-HK" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'cs-2 v. non_cs'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>coef</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'cs-2 v. non_cs'!$I$2:$I$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>5.5000000000000049E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0500000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.0000000000000011E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.2000000000000961E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.5999999999999956E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.6000000000000009E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7.3000000000000009E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'cs-2 v. non_cs'!$H$2:$H$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>5.5000000000000049E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0500000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.0000000000000011E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.799999999999919E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.4000000000000038E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.4000000000000003E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7.6999999999999985E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'cs-2 v. non_cs'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Intercept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C(cs_word_pos_zh)[T.1]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C(cs_word_pos_zh)[T.2]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>word_freq_zh</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cs_word_length_zh</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>sentence_length_zh</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ngram_surp_zh</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'cs-2 v. non_cs'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.44750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.0052000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1174</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.07E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6616-EB48-B430-59BB1A4D7086}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1190201791"/>
+        <c:axId val="1190203439"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1190201791"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1190203439"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1190203439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1190201791"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1708,6 +2191,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2715,6 +3238,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3315,6 +4341,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD92A67A-1A3D-3D48-8D21-29AC1F725262}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97931553-5267-684A-9393-7CEA8AF13D06}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4366,8 +5433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029DC7B5-F4A2-EA4B-AADF-5E0F1302FA20}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4403,30 +5470,30 @@
         <v>6</v>
       </c>
       <c r="B2" s="2">
-        <v>-3.7699999999999997E-2</v>
+        <v>0.55510000000000004</v>
       </c>
       <c r="C2" s="2">
-        <v>1.0999999999999999E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D2" s="2">
-        <v>-3.35</v>
+        <v>193.47499999999999</v>
       </c>
       <c r="E2" s="2">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>-0.06</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G2" s="2">
-        <v>-1.6E-2</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="H2">
         <f>B2-F2</f>
-        <v>2.23E-2</v>
+        <v>5.0999999999999934E-3</v>
       </c>
       <c r="I2">
         <f>G2-B2</f>
-        <v>2.1699999999999997E-2</v>
+        <v>5.9000000000000163E-3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4496,10 +5563,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="2">
-        <v>3.3700000000000001E-2</v>
+        <v>1.0256000000000001</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D5" s="2">
         <v>247.084</v>
@@ -4508,18 +5575,18 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>3.3000000000000002E-2</v>
+        <v>1.0169999999999999</v>
       </c>
       <c r="G5" s="2">
-        <v>3.4000000000000002E-2</v>
+        <v>1.034</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>6.9999999999999923E-4</v>
+        <v>8.6000000000001631E-3</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>3.0000000000000165E-4</v>
+        <v>8.3999999999999631E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4527,10 +5594,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="2">
-        <v>-8.6400000000000005E-2</v>
+        <v>-0.1144</v>
       </c>
       <c r="C6" s="2">
-        <v>3.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="2">
         <v>-27.873000000000001</v>
@@ -4539,18 +5606,18 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>-9.1999999999999998E-2</v>
+        <v>-0.122</v>
       </c>
       <c r="G6" s="2">
-        <v>-0.08</v>
+        <v>-0.106</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>5.5999999999999939E-3</v>
+        <v>7.5999999999999956E-3</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>6.4000000000000029E-3</v>
+        <v>8.4000000000000047E-3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -4558,10 +5625,10 @@
         <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>-1.78E-2</v>
+        <v>-4.4299999999999999E-2</v>
       </c>
       <c r="C7" s="2">
-        <v>1E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D7" s="2">
         <v>-12.122</v>
@@ -4570,18 +5637,277 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>-2.1000000000000001E-2</v>
+        <v>-5.1999999999999998E-2</v>
       </c>
       <c r="G7" s="2">
-        <v>-1.4999999999999999E-2</v>
+        <v>-3.6999999999999998E-2</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>3.2000000000000015E-3</v>
+        <v>7.6999999999999985E-3</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>2.8000000000000004E-3</v>
+        <v>7.3000000000000009E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83C7DF1-9200-9E4E-A0EB-D2FE49CF842E}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.44750000000000001</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>152.15600000000001</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.442</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="H2">
+        <f>B2-F2</f>
+        <v>5.5000000000000049E-3</v>
+      </c>
+      <c r="I2">
+        <f>G2-B2</f>
+        <v>5.5000000000000049E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H8" si="0">B3-F3</f>
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I8" si="1">G3-B3</f>
+        <v>1.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-0.04</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-8.4789999999999992</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-3.1E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>9.0000000000000011E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-1.0052000000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-228.91300000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>-1.014</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-0.997</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>8.799999999999919E-3</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>8.2000000000000961E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.1174</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>29.332000000000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>7.4000000000000038E-3</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>7.5999999999999956E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="F7" s="2">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>7.6000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4.07E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>10.648999999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>7.6999999999999985E-3</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>7.3000000000000009E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>